<commit_message>
Fixed Personalized Abstracts data
</commit_message>
<xml_diff>
--- a/Program/Data/Update/Abstracts_personalized.xlsx
+++ b/Program/Data/Update/Abstracts_personalized.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah\Tugas Akhir\TA\My_Thesis\Program\Data\Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4BBC9233-C7CC-4CBA-9B5F-02A506614C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330BB2E4-9F3F-4780-9CE7-3F7F0134BB61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="372" yWindow="1152" windowWidth="22668" windowHeight="8964" xr2:uid="{629E786C-1A8A-456B-9B6B-B59C086E75E6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
   <si>
     <t>Abstract</t>
   </si>
@@ -183,9 +183,6 @@
   </si>
   <si>
     <t>The world of education system after this COVID19 pandemic will have to change its dimension to map the needs of learners. The proposed framework is focused on transforming the learning experience into two possible ways like online and on-campus learning through groundbreaking agile methodologies. The new interfaces for learners will be included like Gamification, animated tutorial etc. The framework designed here is the outcome of the e-learning experiences of the authors and it tries to add all relevant technologies with cutting-edge research to provide inspirational and transformative knowledge to learners of all ages, social status, communities who form worldwide communities of special-learners. It will rise to the occasion to use its open source technology along with the emerged technologies like IoT, 5G etc, to transcend physical and social borders. This framework is a total learning environment as it will incorporate all possible latest technologies like big data and machine learning. The e-learning system possesses features like personalized e-learning, anomaly detection, student performance monitoring, dynamic content preparations, students' satisfaction monitoring etc. The new framework will include big data, cloud applications, machine learning and artificial intelligence to make the system faster, efficient and smart. The new features will make the e-learning system based on Virtual Smart Total Learning Environment (VSTLE) more technologically sound and efficient in processing, predicting, evaluating and making storage backup. This framework is designed in such a way that the minimum human intervention will be needed for its functioning. As a result, the final output will be more accurate as compared to other e-learning systems available. © 2020 IEEE.</t>
-  </si>
-  <si>
-    <t>[No abstract available]</t>
   </si>
   <si>
     <t>The purpose of this paper is to draw together theories, ideas, and observations related to rewards, motivation, and play to develop and question our understanding and practice of designing reward-based systems and technology. Our exploration includes reinforcement, rewards, motivational theory, flow, play, games, gamification, and machine learning. We examine the design and psychology of reward-based systems in society and technology, using gamification and machine learning as case studies. We propose that the problems that exist with reward-based systems in our society are also present and pertinent when designing technology. We suggest that motivation, exploration, and play are not just fundamental to human learning and behaviour, but that they could transcend nature into machine learning. Finally, we question the value and potential harm of the reward-based systems that permeate every aspect of our lives and assert the importance of ethics in the design of all systems and technology. © 2020 ACM.</t>
@@ -489,13 +486,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -810,16 +806,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AF54513-6EB2-456A-B669-A49A4E9D6F3C}">
-  <dimension ref="A1:A137"/>
+  <dimension ref="A1:A136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:XFD50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="8.88671875" style="3"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -1501,11 +1494,6 @@
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A137" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>